<commit_message>
1st testcase of forgotPassword scenario added
</commit_message>
<xml_diff>
--- a/bin/com/NFHS/xls/Registration.xlsx
+++ b/bin/com/NFHS/xls/Registration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2490" windowWidth="13395" windowHeight="4215" firstSheet="6" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="2490" windowWidth="17850" windowHeight="10680"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="Registration_Account_Setup7" sheetId="13" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:H12"/>
+  <oleSize ref="B7:D8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="48">
   <si>
     <t>TCID</t>
   </si>
@@ -242,12 +242,6 @@
   </si>
   <si>
     <t>skipped</t>
-  </si>
-  <si>
-    <t>fail</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>user4@gmail.com</t>
@@ -734,7 +728,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="B7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -887,7 +881,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="120" x14ac:dyDescent="0.25">
@@ -1362,7 +1356,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1399,10 +1393,10 @@
     </row>
     <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>15</v>
@@ -1414,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>